<commit_message>
Committing for final report
</commit_message>
<xml_diff>
--- a/total uncertainty.xlsx
+++ b/total uncertainty.xlsx
@@ -7,16 +7,21 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="45-100-20" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="45-110-20_1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="45-110-20_2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="45-120-20" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="45-130-20" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="45-70-20" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="45-80-20" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="45-90-20" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="45-100-20_1" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="45-100-20_2" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="45E-100C-20S" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="45E-110C-20S_1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="45E-110C-20S_2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="45E-120C-20S" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="45E-130C-20S" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="40E-100C-20S" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="50E-100C-20S" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="30E-100C-20S" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="10E-100C-20S" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="20E-100C-20S" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="45E-70C-20S" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="45E-80C-20S" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="45E-90C-20S" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="45E-100C-20S_1" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="45E-100C-20S_2" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -394,10 +399,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.003634001285426501</v>
+        <v>0.005404306017488518</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3750176075404227</v>
+        <v>0.3750389400096084</v>
       </c>
     </row>
     <row r="3">
@@ -407,10 +412,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.003718714095629548</v>
+        <v>0.009590664700019288</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2000345690987561</v>
+        <v>0.2002298200802972</v>
       </c>
     </row>
     <row r="4">
@@ -420,10 +425,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.003712024237385222</v>
+        <v>0.008974513425979465</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3750183717152253</v>
+        <v>0.3751073738161289</v>
       </c>
     </row>
   </sheetData>
@@ -464,6 +469,356 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>0.009845298438637472</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3751292176055417</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Tsuc</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.01851916449292662</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.2008555686395478</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Pdis</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.01698336445696131</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3753843825577697</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Psuc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.005971066379745952</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3750475351654925</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Tsuc</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.009247418945231697</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.2002136727527584</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Pdis</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.004027294267447297</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3750216248419771</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Psuc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.002282389966956758</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3750069456742918</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Tsuc</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.002947503191030469</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.200021718258446</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Pdis</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.01097448805234708</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3751605514816438</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Psuc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.00326902538528967</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3750142484319358</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Tsuc</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.004563948699437166</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.2000520672918206</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Pdis</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.004671511653535377</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3750290962327179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Psuc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.00689705771944537</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3750634205106989</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Tsuc</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.009382206823771232</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.2002199435742704</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Pdis</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.01069394072554172</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3751524495031872</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Psuc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>0.003204072335951327</v>
       </c>
       <c r="C2" t="n">
@@ -814,10 +1169,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.005971066379745952</v>
+        <v>0.003180036000948107</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3750475351654925</v>
+        <v>0.3750134832628919</v>
       </c>
     </row>
     <row r="3">
@@ -827,10 +1182,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.009247418945231697</v>
+        <v>0.004248031915951518</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2002136727527584</v>
+        <v>0.2000451093507636</v>
       </c>
     </row>
     <row r="4">
@@ -840,10 +1195,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.004027294267447297</v>
+        <v>0.004174083028707757</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3750216248419771</v>
+        <v>0.3750232299060027</v>
       </c>
     </row>
   </sheetData>
@@ -884,10 +1239,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.002282389966956758</v>
+        <v>0.006637593619131832</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3750069456742918</v>
+        <v>0.3750587389317209</v>
       </c>
     </row>
     <row r="3">
@@ -897,10 +1252,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.002947503191030469</v>
+        <v>0.009236408910930782</v>
       </c>
       <c r="C3" t="n">
-        <v>0.200021718258446</v>
+        <v>0.2002131645261368</v>
       </c>
     </row>
     <row r="4">
@@ -910,10 +1265,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01097448805234708</v>
+        <v>0.009937420531255632</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3751605514816438</v>
+        <v>0.3751316466612954</v>
       </c>
     </row>
   </sheetData>
@@ -954,10 +1309,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.00326902538528967</v>
+        <v>0.009952596682775367</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3750142484319358</v>
+        <v>0.375132048991725</v>
       </c>
     </row>
     <row r="3">
@@ -967,10 +1322,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.004563948699437166</v>
+        <v>0.0189407108509347</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2000520672918206</v>
+        <v>0.200894874318731</v>
       </c>
     </row>
     <row r="4">
@@ -980,10 +1335,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.004671511653535377</v>
+        <v>0.0164669993420788</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3750290962327179</v>
+        <v>0.3753613753002991</v>
       </c>
     </row>
   </sheetData>
@@ -1024,10 +1379,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.00689705771944537</v>
+        <v>0.009770259028067965</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3750634205106989</v>
+        <v>0.3751272556899532</v>
       </c>
     </row>
     <row r="3">
@@ -1037,10 +1392,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.009382206823771232</v>
+        <v>0.01956201438325054</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2002199435742704</v>
+        <v>0.2009544038002913</v>
       </c>
     </row>
     <row r="4">
@@ -1050,10 +1405,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01069394072554172</v>
+        <v>0.02422291349862557</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3751524495031872</v>
+        <v>0.3757815183565604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>